<commit_message>
add results/code for rq*
</commit_message>
<xml_diff>
--- a/rq3/results/rq3_results.xlsx
+++ b/rq3/results/rq3_results.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lgk/git/uni/web_test_generation/near-duplicate-detection/rq3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lgk/git/uni/web_test_generation/near-duplicate-detection/rq3/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7D978F-979D-0646-8829-3220935F77AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA16AB2E-12E5-3C4C-9227-03D545881F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4780" yWindow="3680" windowWidth="27240" windowHeight="16440" xr2:uid="{ACC9B923-10F0-1147-8CB8-5D2CBDE7790A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -105,7 +105,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,26 +134,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -163,9 +143,22 @@
     <font>
       <b/>
       <sz val="20"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -176,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -255,78 +248,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,7 +619,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,117 +628,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="21"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>7.2</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="4">
         <v>7.4</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="4">
         <v>7.1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="4">
         <v>4.96</v>
       </c>
-      <c r="F3" s="12">
-        <v>13.94</v>
-      </c>
-      <c r="G3" s="14">
+      <c r="F3" s="4">
+        <v>6.9</v>
+      </c>
+      <c r="G3" s="10">
         <v>6.53</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="4">
         <v>7.4</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="4">
         <v>7.14</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="4">
         <v>6.57</v>
       </c>
       <c r="K3" s="11">
-        <v>14.06</v>
-      </c>
+        <v>7.1</v>
+      </c>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="11"/>
-      <c r="L4" t="s">
+      <c r="L4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="15">
         <v>15.66</v>
       </c>
       <c r="C5" s="13">
@@ -795,10 +753,10 @@
       <c r="E5" s="13">
         <v>15.66</v>
       </c>
-      <c r="F5" s="12">
-        <v>17.440000000000001</v>
-      </c>
-      <c r="G5" s="14">
+      <c r="F5" s="13">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G5" s="15">
         <v>19.3</v>
       </c>
       <c r="H5" s="13">
@@ -810,18 +768,19 @@
       <c r="J5" s="13">
         <v>19.399999999999999</v>
       </c>
-      <c r="K5" s="11">
-        <v>23.08</v>
-      </c>
+      <c r="K5" s="16">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="15">
         <v>15.37</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <v>17.63</v>
       </c>
       <c r="D6" s="13">
@@ -830,10 +789,10 @@
       <c r="E6" s="13">
         <v>17.600000000000001</v>
       </c>
-      <c r="F6" s="12">
-        <v>8.75</v>
-      </c>
-      <c r="G6" s="14">
+      <c r="F6" s="13">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G6" s="15">
         <v>19.559999999999999</v>
       </c>
       <c r="H6" s="13">
@@ -845,15 +804,16 @@
       <c r="J6" s="13">
         <v>17.600000000000001</v>
       </c>
-      <c r="K6" s="11">
-        <v>9.17</v>
-      </c>
+      <c r="K6" s="16">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="15">
         <v>7.62</v>
       </c>
       <c r="C7" s="13">
@@ -865,10 +825,10 @@
       <c r="E7" s="13">
         <v>7.63</v>
       </c>
-      <c r="F7" s="12">
-        <v>7.36</v>
-      </c>
-      <c r="G7" s="14">
+      <c r="F7" s="13">
+        <v>7.4</v>
+      </c>
+      <c r="G7" s="15">
         <v>7.21</v>
       </c>
       <c r="H7" s="13">
@@ -880,28 +840,29 @@
       <c r="J7" s="13">
         <v>7.6</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="16">
         <v>7.5</v>
       </c>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="15">
         <v>26.9</v>
       </c>
       <c r="C8" s="13">
         <v>25.3</v>
       </c>
-      <c r="D8" s="12">
-        <v>13.46</v>
-      </c>
-      <c r="E8" s="12">
-        <v>13.78</v>
-      </c>
-      <c r="F8" s="12">
-        <v>13.78</v>
+      <c r="D8" s="13">
+        <v>13.5</v>
+      </c>
+      <c r="E8" s="13">
+        <v>13.8</v>
+      </c>
+      <c r="F8" s="13">
+        <v>13.8</v>
       </c>
       <c r="G8" s="15">
         <v>25.6</v>
@@ -909,171 +870,172 @@
       <c r="H8" s="13">
         <v>41.6</v>
       </c>
-      <c r="I8" s="12">
-        <v>13.46</v>
-      </c>
-      <c r="J8" s="12">
-        <v>13.78</v>
-      </c>
-      <c r="K8" s="11">
-        <v>13.78</v>
-      </c>
+      <c r="I8" s="13">
+        <v>13.5</v>
+      </c>
+      <c r="J8" s="13">
+        <v>13.8</v>
+      </c>
+      <c r="K8" s="16">
+        <v>13.8</v>
+      </c>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="15">
         <v>54</v>
       </c>
       <c r="C9" s="13">
         <v>58.4</v>
       </c>
-      <c r="D9" s="12">
-        <v>56.51</v>
-      </c>
-      <c r="E9" s="12">
-        <v>56.11</v>
-      </c>
-      <c r="F9" s="12">
-        <v>55.57</v>
-      </c>
-      <c r="G9" s="14">
+      <c r="D9" s="13">
+        <v>56.5</v>
+      </c>
+      <c r="E9" s="13">
+        <v>56.1</v>
+      </c>
+      <c r="F9" s="13">
+        <v>55.6</v>
+      </c>
+      <c r="G9" s="15">
         <v>54.7</v>
       </c>
       <c r="H9" s="13">
         <v>59.8</v>
       </c>
-      <c r="I9" s="12">
-        <v>58.11</v>
-      </c>
-      <c r="J9" s="12">
-        <v>56.98</v>
-      </c>
-      <c r="K9" s="11">
-        <v>55.67</v>
-      </c>
+      <c r="I9" s="13">
+        <v>58.1</v>
+      </c>
+      <c r="J9" s="13">
+        <v>57</v>
+      </c>
+      <c r="K9" s="16">
+        <v>55.7</v>
+      </c>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="15">
         <v>30.1</v>
       </c>
       <c r="C10" s="13">
         <v>29.6</v>
       </c>
-      <c r="D10" s="12">
-        <v>29.06</v>
-      </c>
-      <c r="E10" s="12">
-        <v>28.78</v>
-      </c>
-      <c r="F10" s="12">
-        <v>28.78</v>
-      </c>
-      <c r="G10" s="14">
+      <c r="D10" s="13">
+        <v>29.1</v>
+      </c>
+      <c r="E10" s="13">
+        <v>28.8</v>
+      </c>
+      <c r="F10" s="13">
+        <v>28.8</v>
+      </c>
+      <c r="G10" s="15">
         <v>30.9</v>
       </c>
       <c r="H10" s="13">
         <v>30.9</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="13">
         <v>29.6</v>
       </c>
-      <c r="J10" s="12">
-        <v>30.74</v>
-      </c>
-      <c r="K10" s="11">
-        <v>30.74</v>
-      </c>
+      <c r="J10" s="13">
+        <v>30.7</v>
+      </c>
+      <c r="K10" s="16">
+        <v>30.7</v>
+      </c>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="17">
         <v>32.700000000000003</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="18">
         <v>32.200000000000003</v>
       </c>
-      <c r="D11" s="7">
-        <v>31.94</v>
-      </c>
-      <c r="E11" s="7">
-        <v>32.11</v>
-      </c>
-      <c r="F11" s="7">
-        <v>32.11</v>
-      </c>
-      <c r="G11" s="9">
+      <c r="D11" s="18">
+        <v>31.9</v>
+      </c>
+      <c r="E11" s="18">
+        <v>32.1</v>
+      </c>
+      <c r="F11" s="18">
+        <v>32.1</v>
+      </c>
+      <c r="G11" s="17">
         <v>32.299999999999997</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="18">
         <v>31.8</v>
       </c>
-      <c r="I11" s="7">
-        <v>33.44</v>
-      </c>
-      <c r="J11" s="7">
-        <v>32.42</v>
-      </c>
-      <c r="K11" s="6">
-        <v>32.11</v>
-      </c>
+      <c r="I11" s="18">
+        <v>33.4</v>
+      </c>
+      <c r="J11" s="18">
+        <v>32.4</v>
+      </c>
+      <c r="K11" s="19">
+        <v>32.1</v>
+      </c>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="13">
         <f>AVERAGE(B3:B11)</f>
         <v>23.693750000000001</v>
       </c>
-      <c r="C12" s="2">
-        <f>AVERAGE(C3:C11)</f>
+      <c r="C12" s="14">
+        <f t="shared" ref="C12:K12" si="0">AVERAGE(C3:C11)</f>
         <v>24.664999999999999</v>
       </c>
-      <c r="D12" s="1">
-        <f>AVERAGE(D3:D11)</f>
-        <v>22.46</v>
-      </c>
-      <c r="E12" s="1">
-        <f>AVERAGE(E3:E11)</f>
-        <v>22.078749999999999</v>
-      </c>
-      <c r="F12" s="1">
-        <f>AVERAGE(F3:F11)</f>
-        <v>22.216250000000002</v>
-      </c>
-      <c r="G12" s="3">
-        <f>AVERAGE(G3:G11)</f>
+      <c r="D12" s="13">
+        <f t="shared" si="0"/>
+        <v>22.463750000000001</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="0"/>
+        <v>22.081250000000001</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="0"/>
+        <v>21.35</v>
+      </c>
+      <c r="G12" s="15">
+        <f t="shared" si="0"/>
         <v>24.512500000000003</v>
       </c>
-      <c r="H12" s="2">
-        <f>AVERAGE(H3:H11)</f>
+      <c r="H12" s="14">
+        <f t="shared" si="0"/>
         <v>26.663750000000004</v>
       </c>
-      <c r="I12" s="1">
-        <f>AVERAGE(I3:I11)</f>
-        <v>23.358750000000001</v>
-      </c>
-      <c r="J12" s="1">
-        <f>AVERAGE(J3:J11)</f>
-        <v>23.136250000000004</v>
-      </c>
-      <c r="K12" s="1">
-        <f>AVERAGE(K3:K11)</f>
-        <v>23.263750000000002</v>
-      </c>
+      <c r="I12" s="13">
+        <f t="shared" si="0"/>
+        <v>23.357500000000002</v>
+      </c>
+      <c r="J12" s="13">
+        <f t="shared" si="0"/>
+        <v>23.133749999999999</v>
+      </c>
+      <c r="K12" s="13">
+        <f t="shared" si="0"/>
+        <v>21.9</v>
+      </c>
+      <c r="L12" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>